<commit_message>
updated test for add user
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Keyword</t>
   </si>
@@ -71,6 +71,57 @@
   </si>
   <si>
     <t>userbtn</t>
+  </si>
+  <si>
+    <t>Read User Table</t>
+  </si>
+  <si>
+    <t>Add user</t>
+  </si>
+  <si>
+    <t>addUser</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>mangesh</t>
+  </si>
+  <si>
+    <t>mangesh@gmail.com</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>SELECTVALUE</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>ALERTHANDLE</t>
   </si>
 </sst>
 </file>
@@ -127,17 +178,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +556,7 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -539,30 +589,186 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <v>7894561230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>